<commit_message>
included mtm derived from orders & option chain prices
</commit_message>
<xml_diff>
--- a/volbacktest/simulationData.xlsx
+++ b/volbacktest/simulationData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="202">
   <si>
     <t>AccountCode_</t>
   </si>
@@ -592,9 +592,6 @@
   </si>
   <si>
     <t>-133.92</t>
-  </si>
-  <si>
-    <t>20160920154202</t>
   </si>
   <si>
     <t>4.3317</t>
@@ -713,7 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -727,6 +724,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1078,13 +1076,13 @@
         <v>97</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1102,7 +1100,7 @@
   <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1672,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4:AH7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2288,15 +2286,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2324,11 +2323,11 @@
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>176</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>237606530</v>
       </c>
@@ -2428,7 +2427,7 @@
         <v>185</v>
       </c>
       <c r="J2" s="6">
-        <v>-560.4</v>
+        <v>-550.4</v>
       </c>
       <c r="K2" t="s">
         <v>111</v>
@@ -2460,17 +2459,21 @@
       <c r="V2" t="s">
         <v>189</v>
       </c>
-      <c r="W2" t="s">
-        <v>65</v>
-      </c>
-      <c r="X2" t="s">
-        <v>190</v>
+      <c r="W2">
+        <v>20160919</v>
+      </c>
+      <c r="X2" s="7">
+        <v>20160919214202</v>
       </c>
       <c r="Y2" s="3">
-        <v>42633.654166666704</v>
+        <v>42632.903541666703</v>
+      </c>
+      <c r="Z2">
+        <f>L2*C2</f>
+        <v>-426.47920049999999</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>237606550</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" t="s">
         <v>101</v>
@@ -2493,10 +2496,10 @@
         <v>112</v>
       </c>
       <c r="I3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J3" s="6">
-        <v>90.47</v>
+        <v>95.47</v>
       </c>
       <c r="K3" t="s">
         <v>111</v>
@@ -2526,19 +2529,23 @@
         <v>101</v>
       </c>
       <c r="V3" t="s">
-        <v>193</v>
-      </c>
-      <c r="W3" t="s">
-        <v>65</v>
-      </c>
-      <c r="X3" t="s">
-        <v>190</v>
+        <v>192</v>
+      </c>
+      <c r="W3">
+        <v>20160919</v>
+      </c>
+      <c r="X3" s="7">
+        <v>20160919214202</v>
       </c>
       <c r="Y3" s="3">
-        <v>42633.654166666704</v>
+        <v>42632.903541666703</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z9" si="0">L3*C3</f>
+        <v>129.95099999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>237606986</v>
       </c>
@@ -2546,7 +2553,7 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E4" t="s">
         <v>101</v>
@@ -2561,10 +2568,10 @@
         <v>137</v>
       </c>
       <c r="I4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J4" s="6">
-        <v>1199.81</v>
+        <v>1159.81</v>
       </c>
       <c r="K4" t="s">
         <v>111</v>
@@ -2594,19 +2601,23 @@
         <v>101</v>
       </c>
       <c r="V4" t="s">
-        <v>196</v>
-      </c>
-      <c r="W4" t="s">
-        <v>65</v>
-      </c>
-      <c r="X4" t="s">
-        <v>190</v>
+        <v>195</v>
+      </c>
+      <c r="W4">
+        <v>20160919</v>
+      </c>
+      <c r="X4" s="7">
+        <v>20160919214202</v>
       </c>
       <c r="Y4" s="3">
-        <v>42633.654166666704</v>
+        <v>42632.903541666703</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>1329.3510000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>237607006</v>
       </c>
@@ -2614,7 +2625,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" t="s">
         <v>101</v>
@@ -2629,10 +2640,10 @@
         <v>131</v>
       </c>
       <c r="I5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J5" s="6">
-        <v>-2009.71</v>
+        <v>-2059.71</v>
       </c>
       <c r="K5" t="s">
         <v>111</v>
@@ -2662,22 +2673,316 @@
         <v>101</v>
       </c>
       <c r="V5" t="s">
-        <v>199</v>
-      </c>
-      <c r="W5" t="s">
-        <v>65</v>
-      </c>
-      <c r="X5" t="s">
+        <v>198</v>
+      </c>
+      <c r="W5">
+        <v>20160919</v>
+      </c>
+      <c r="X5" s="7">
+        <v>20160919214202</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>42632.903541666703</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>-2174.5413000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <f>A2+100</f>
+        <v>237606630</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" t="s">
+        <v>185</v>
+      </c>
+      <c r="J6" s="6">
+        <v>-560.4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L6" t="s">
+        <v>186</v>
+      </c>
+      <c r="M6" t="s">
+        <v>187</v>
+      </c>
+      <c r="N6" t="s">
+        <v>115</v>
+      </c>
+      <c r="O6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R6" t="s">
+        <v>188</v>
+      </c>
+      <c r="S6" t="s">
+        <v>119</v>
+      </c>
+      <c r="T6" t="s">
+        <v>103</v>
+      </c>
+      <c r="U6" t="s">
+        <v>101</v>
+      </c>
+      <c r="V6" t="s">
+        <v>189</v>
+      </c>
+      <c r="W6">
+        <v>20160920</v>
+      </c>
+      <c r="X6" s="7">
+        <v>20160920154202</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>42633.654166666704</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="0"/>
+        <v>-426.47920049999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <f t="shared" ref="A7:A9" si="1">A3+100</f>
+        <v>237606650</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
         <v>190</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="E7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I7" t="s">
+        <v>191</v>
+      </c>
+      <c r="J7" s="6">
+        <v>90.47</v>
+      </c>
+      <c r="K7" t="s">
+        <v>111</v>
+      </c>
+      <c r="L7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" t="s">
+        <v>187</v>
+      </c>
+      <c r="N7" t="s">
+        <v>115</v>
+      </c>
+      <c r="O7" t="s">
+        <v>107</v>
+      </c>
+      <c r="R7" t="s">
+        <v>188</v>
+      </c>
+      <c r="S7" t="s">
+        <v>104</v>
+      </c>
+      <c r="T7" t="s">
+        <v>103</v>
+      </c>
+      <c r="U7" t="s">
+        <v>101</v>
+      </c>
+      <c r="V7" t="s">
+        <v>192</v>
+      </c>
+      <c r="W7">
+        <v>20160920</v>
+      </c>
+      <c r="X7" s="7">
+        <v>20160920154202</v>
+      </c>
+      <c r="Y7" s="3">
         <v>42633.654166666704</v>
       </c>
+      <c r="Z7">
+        <f t="shared" si="0"/>
+        <v>129.95099999999999</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="J6" s="6"/>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <f t="shared" si="1"/>
+        <v>237607086</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H8" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" t="s">
+        <v>194</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1199.81</v>
+      </c>
+      <c r="K8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" t="s">
+        <v>187</v>
+      </c>
+      <c r="N8" t="s">
+        <v>115</v>
+      </c>
+      <c r="O8" t="s">
+        <v>128</v>
+      </c>
+      <c r="R8" t="s">
+        <v>188</v>
+      </c>
+      <c r="S8" t="s">
+        <v>135</v>
+      </c>
+      <c r="T8" t="s">
+        <v>103</v>
+      </c>
+      <c r="U8" t="s">
+        <v>101</v>
+      </c>
+      <c r="V8" t="s">
+        <v>195</v>
+      </c>
+      <c r="W8">
+        <v>20160920</v>
+      </c>
+      <c r="X8" s="7">
+        <v>20160920154202</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>42633.654166666704</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="0"/>
+        <v>1329.3510000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <f t="shared" si="1"/>
+        <v>237607106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I9" t="s">
+        <v>197</v>
+      </c>
+      <c r="J9" s="6">
+        <v>-2009.71</v>
+      </c>
+      <c r="K9" t="s">
+        <v>111</v>
+      </c>
+      <c r="L9" t="s">
+        <v>186</v>
+      </c>
+      <c r="M9" t="s">
+        <v>187</v>
+      </c>
+      <c r="N9" t="s">
+        <v>115</v>
+      </c>
+      <c r="O9" t="s">
+        <v>128</v>
+      </c>
+      <c r="R9" t="s">
+        <v>188</v>
+      </c>
+      <c r="S9" t="s">
+        <v>126</v>
+      </c>
+      <c r="T9" t="s">
+        <v>103</v>
+      </c>
+      <c r="U9" t="s">
+        <v>101</v>
+      </c>
+      <c r="V9" t="s">
+        <v>198</v>
+      </c>
+      <c r="W9">
+        <v>20160920</v>
+      </c>
+      <c r="X9" s="7">
+        <v>20160920154202</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>42633.654166666704</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="0"/>
+        <v>-2174.5413000000003</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test done with base case and scenario run analytics from simple strategy in h5
</commit_message>
<xml_diff>
--- a/volbacktest/simulationData.xlsx
+++ b/volbacktest/simulationData.xlsx
@@ -9,20 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="2" r:id="rId1"/>
     <sheet name="account_spy1016dls" sheetId="1" r:id="rId2"/>
     <sheet name="orders_spy1016dls" sheetId="3" r:id="rId3"/>
     <sheet name="portfolio_spy1016dls" sheetId="4" r:id="rId4"/>
+    <sheet name="account_spy1016wild" sheetId="5" r:id="rId5"/>
+    <sheet name="orders_spy1016wild" sheetId="6" r:id="rId6"/>
+    <sheet name="portfolio_spy1016wild" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="125">
   <si>
     <t>AccountCode_</t>
   </si>
@@ -385,6 +388,18 @@
   </si>
   <si>
     <t>en portfolio hay que meter un registro por cada hora con orders</t>
+  </si>
+  <si>
+    <t>SPY OCT16 wild test</t>
+  </si>
+  <si>
+    <t>spy1016wild</t>
+  </si>
+  <si>
+    <t>20161017214106</t>
+  </si>
+  <si>
+    <t>20161017  21:29:22</t>
   </si>
 </sst>
 </file>
@@ -425,7 +440,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,6 +456,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,7 +500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -492,18 +513,35 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -811,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,8 +902,19 @@
         <v>115</v>
       </c>
     </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" t="s">
+        <v>122</v>
+      </c>
+    </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="12" t="s">
         <v>116</v>
       </c>
     </row>
@@ -891,67 +940,67 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="14" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="14" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="14" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="17" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="18" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="K19" s="12" t="s">
+      <c r="K19" s="14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="20" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="K20" s="12" t="s">
+      <c r="K20" s="14" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="21" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="14" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="K22" s="12" t="s">
+      <c r="K22" s="14" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="23" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="K23" s="12" t="s">
+      <c r="K23" s="14" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="24" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="K24" s="12" t="s">
+      <c r="K24" s="14" t="s">
         <v>73</v>
       </c>
     </row>
@@ -977,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1020,94 +1069,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="11" t="s">
         <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
@@ -1127,89 +1176,89 @@
       <c r="A2" s="2">
         <v>42632.654236111099</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="8" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
       <c r="AD2" t="s">
         <v>37</v>
       </c>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42632.950763888897</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="8" t="s">
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
       <c r="AD3" t="s">
         <v>38</v>
       </c>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="7"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1261,97 +1310,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="11" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1359,43 +1408,43 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="8"/>
       <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
       <c r="H2" t="s">
         <v>36</v>
       </c>
       <c r="I2" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
       <c r="M2" t="s">
         <v>55</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
       <c r="P2" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
       <c r="S2" t="s">
         <v>71</v>
       </c>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
       <c r="V2" t="s">
         <v>63</v>
       </c>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
       <c r="Y2" t="s">
         <v>68</v>
       </c>
@@ -1411,7 +1460,7 @@
       <c r="AC2" t="s">
         <v>67</v>
       </c>
-      <c r="AD2" s="7"/>
+      <c r="AD2" s="8"/>
       <c r="AE2" s="3">
         <v>42632.903541666703</v>
       </c>
@@ -1420,43 +1469,43 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="8"/>
       <c r="C3" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" t="s">
         <v>36</v>
       </c>
       <c r="I3" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
       <c r="M3" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
       <c r="P3" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
       <c r="S3" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
       <c r="V3" t="s">
         <v>63</v>
       </c>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
       <c r="Y3" t="s">
         <v>68</v>
       </c>
@@ -1472,7 +1521,7 @@
       <c r="AC3" t="s">
         <v>67</v>
       </c>
-      <c r="AD3" s="7"/>
+      <c r="AD3" s="8"/>
       <c r="AE3" s="3">
         <v>42632.903541666703</v>
       </c>
@@ -1481,43 +1530,43 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" t="s">
         <v>36</v>
       </c>
       <c r="I4" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
       <c r="M4" t="s">
         <v>55</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
       <c r="P4" t="s">
         <v>54</v>
       </c>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
       <c r="S4" t="s">
         <v>66</v>
       </c>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
       <c r="V4" t="s">
         <v>63</v>
       </c>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
       <c r="Y4" t="s">
         <v>62</v>
       </c>
@@ -1533,7 +1582,7 @@
       <c r="AC4" t="s">
         <v>60</v>
       </c>
-      <c r="AD4" s="7"/>
+      <c r="AD4" s="8"/>
       <c r="AE4" s="3">
         <v>42632.903541666703</v>
       </c>
@@ -1542,43 +1591,43 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" t="s">
         <v>36</v>
       </c>
       <c r="I5" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
       <c r="M5" t="s">
         <v>55</v>
       </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
       <c r="P5" t="s">
         <v>54</v>
       </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
       <c r="S5" t="s">
         <v>64</v>
       </c>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
       <c r="V5" t="s">
         <v>63</v>
       </c>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
       <c r="Y5" t="s">
         <v>62</v>
       </c>
@@ -1594,7 +1643,7 @@
       <c r="AC5" t="s">
         <v>60</v>
       </c>
-      <c r="AD5" s="7"/>
+      <c r="AD5" s="8"/>
       <c r="AE5" s="3">
         <v>42632.903541666703</v>
       </c>
@@ -1603,43 +1652,43 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="8"/>
       <c r="C6" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" t="s">
         <v>36</v>
       </c>
       <c r="I6" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
       <c r="M6" t="s">
         <v>55</v>
       </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
       <c r="P6" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
       <c r="S6" t="s">
         <v>59</v>
       </c>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
       <c r="V6" t="s">
         <v>52</v>
       </c>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
       <c r="Y6" t="s">
         <v>51</v>
       </c>
@@ -1655,7 +1704,7 @@
       <c r="AC6" t="s">
         <v>47</v>
       </c>
-      <c r="AD6" s="7"/>
+      <c r="AD6" s="8"/>
       <c r="AE6" s="3">
         <v>42632.903541666703</v>
       </c>
@@ -1664,43 +1713,43 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="8"/>
       <c r="C7" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
       <c r="H7" t="s">
         <v>36</v>
       </c>
       <c r="I7" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
       <c r="M7" t="s">
         <v>55</v>
       </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
       <c r="P7" t="s">
         <v>54</v>
       </c>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
       <c r="S7" t="s">
         <v>53</v>
       </c>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
       <c r="V7" t="s">
         <v>52</v>
       </c>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
       <c r="Y7" t="s">
         <v>51</v>
       </c>
@@ -1716,7 +1765,7 @@
       <c r="AC7" t="s">
         <v>47</v>
       </c>
-      <c r="AD7" s="7"/>
+      <c r="AD7" s="8"/>
       <c r="AE7" s="3">
         <v>42632.903541666703</v>
       </c>
@@ -1732,7 +1781,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1765,77 +1814,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="11"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="11" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1843,21 +1892,21 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
       <c r="G2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8">
         <v>0.18680089999999999</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="15">
         <v>-550</v>
       </c>
       <c r="K2">
@@ -1866,26 +1915,26 @@
       <c r="L2">
         <v>-30</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
       <c r="O2" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
       <c r="S2" t="s">
         <v>57</v>
       </c>
       <c r="T2" t="s">
         <v>48</v>
       </c>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
       <c r="W2">
         <v>20160919</v>
       </c>
-      <c r="X2" s="6">
+      <c r="X2" s="7">
         <v>20160919214202</v>
       </c>
       <c r="Y2" s="3">
@@ -1896,21 +1945,21 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="G3" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8">
         <v>3.01575E-2</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="15">
         <v>95.47</v>
       </c>
       <c r="K3">
@@ -1919,26 +1968,26 @@
       <c r="L3">
         <v>30</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
       <c r="O3" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
       <c r="S3" t="s">
         <v>49</v>
       </c>
       <c r="T3" t="s">
         <v>48</v>
       </c>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
       <c r="W3">
         <v>20160919</v>
       </c>
-      <c r="X3" s="6">
+      <c r="X3" s="7">
         <v>20160919214202</v>
       </c>
       <c r="Y3" s="3">
@@ -1949,21 +1998,21 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
       <c r="G4" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7">
+      <c r="H4" s="8"/>
+      <c r="I4" s="8">
         <v>0.39993784999999998</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="15">
         <v>1159.81</v>
       </c>
       <c r="K4">
@@ -1972,26 +2021,26 @@
       <c r="L4">
         <v>30</v>
       </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
       <c r="O4" t="s">
         <v>63</v>
       </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
       <c r="S4" t="s">
         <v>65</v>
       </c>
       <c r="T4" t="s">
         <v>48</v>
       </c>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
       <c r="W4">
         <v>20160919</v>
       </c>
-      <c r="X4" s="6">
+      <c r="X4" s="7">
         <v>20160919214202</v>
       </c>
       <c r="Y4" s="3">
@@ -2002,21 +2051,21 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
       <c r="G5" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7">
+      <c r="H5" s="8"/>
+      <c r="I5" s="8">
         <v>0.66990495000000005</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="15">
         <v>-2059.71</v>
       </c>
       <c r="K5">
@@ -2025,30 +2074,1468 @@
       <c r="L5">
         <v>-30</v>
       </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
       <c r="O5" t="s">
         <v>63</v>
       </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
       <c r="S5" t="s">
         <v>61</v>
       </c>
       <c r="T5" t="s">
         <v>48</v>
       </c>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
       <c r="W5">
         <v>20160919</v>
       </c>
-      <c r="X5" s="6">
+      <c r="X5" s="7">
         <v>20160919214202</v>
       </c>
       <c r="Y5" s="3">
         <v>42632.903541666703</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="17" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="22.88671875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="19.77734375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="22.109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="22" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="19.88671875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="23.21875" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="17.77734375" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="21.33203125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="20.33203125" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="20.44140625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="18.44140625" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.5546875" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="21.88671875" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="23.88671875" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.77734375" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="20.6640625" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="17.33203125" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="19" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>42632.654236111099</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2">
+        <v>4397.4399999999996</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8">
+        <v>1009712.29</v>
+      </c>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>42632.950763888897</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3">
+        <v>19397.439999999999</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8">
+        <v>1010845.02</v>
+      </c>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A4" s="21">
+        <v>42660.654236111113</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9">
+        <v>19397.439999999999</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="8">
+        <v>1010845.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A5" s="21">
+        <v>42660.95076388889</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9">
+        <v>19397.439999999999</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="8">
+        <f>AD4+1000</f>
+        <v>1011845.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" customWidth="1"/>
+    <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="6.21875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="20.44140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="10" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5546875" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="3.77734375" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.33203125" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="9.44140625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.33203125" customWidth="1"/>
+    <col min="28" max="28" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE1" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8">
+        <v>0.439</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2">
+        <v>27</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2">
+        <v>195</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="25">
+        <v>42632.903541666703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8">
+        <v>0.73</v>
+      </c>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3">
+        <v>27</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA3">
+        <v>200</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="25">
+        <v>42632.903541666703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8">
+        <v>0.43</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8">
+        <v>0.43</v>
+      </c>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" t="s">
+        <v>63</v>
+      </c>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4">
+        <v>3</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA4">
+        <v>195</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="25">
+        <v>42632.903541666703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8">
+        <v>0.72</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8">
+        <v>0.72</v>
+      </c>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" t="s">
+        <v>63</v>
+      </c>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5">
+        <v>3</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA5">
+        <v>200</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="25">
+        <v>42632.903541666703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6">
+        <v>100</v>
+      </c>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" t="s">
+        <v>52</v>
+      </c>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6">
+        <v>30</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA6">
+        <v>223</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="25">
+        <v>42632.903541666703</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7">
+        <v>100</v>
+      </c>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" t="s">
+        <v>52</v>
+      </c>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7">
+        <v>30</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA7">
+        <v>228</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="25">
+        <v>42632.903541666703</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="24">
+        <v>20161017</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9">
+        <v>100</v>
+      </c>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>195</v>
+      </c>
+      <c r="AB8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC8" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="25">
+        <v>42660.903541666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5546875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.77734375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="7.77734375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5546875" customWidth="1"/>
+    <col min="20" max="20" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="13" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" s="13"/>
+      <c r="B1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2">
+        <v>14.215973350000001</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8">
+        <v>0.18680089999999999</v>
+      </c>
+      <c r="J2" s="15">
+        <v>-550</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2">
+        <v>-30</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="6">
+        <v>223</v>
+      </c>
+      <c r="T2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2">
+        <v>20160919</v>
+      </c>
+      <c r="X2" s="7">
+        <v>20160919214202</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>42632.903541666703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3">
+        <v>4.3316999999999997</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8">
+        <v>3.01575E-2</v>
+      </c>
+      <c r="J3" s="15">
+        <v>95.47</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>30</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="6">
+        <v>228</v>
+      </c>
+      <c r="T3" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3">
+        <v>20160919</v>
+      </c>
+      <c r="X3" s="7">
+        <v>20160919214202</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>42632.903541666703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4">
+        <v>44.311700000000002</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8">
+        <v>0.39993784999999998</v>
+      </c>
+      <c r="J4" s="15">
+        <v>1159.81</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>30</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="6">
+        <v>195</v>
+      </c>
+      <c r="T4" t="s">
+        <v>48</v>
+      </c>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4">
+        <v>20160919</v>
+      </c>
+      <c r="X4" s="7">
+        <v>20160919214202</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>42632.903541666703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5">
+        <v>72.484710000000007</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8">
+        <v>0.66990495000000005</v>
+      </c>
+      <c r="J5" s="15">
+        <v>-2059.71</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>-30</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="6">
+        <v>200</v>
+      </c>
+      <c r="T5" t="s">
+        <v>48</v>
+      </c>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5">
+        <v>20160919</v>
+      </c>
+      <c r="X5" s="7">
+        <v>20160919214202</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>42632.903541666703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9">
+        <v>14.215973350000001</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
+        <v>0.18680089999999999</v>
+      </c>
+      <c r="J6" s="22">
+        <v>-550</v>
+      </c>
+      <c r="K6" s="9">
+        <v>100</v>
+      </c>
+      <c r="L6" s="9">
+        <v>-30</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="22">
+        <v>223</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9">
+        <v>20161017</v>
+      </c>
+      <c r="X6" s="23">
+        <v>20161017214202</v>
+      </c>
+      <c r="Y6" s="20">
+        <v>42660.903541666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9">
+        <v>4.3316999999999997</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9">
+        <v>3.01575E-2</v>
+      </c>
+      <c r="J7" s="22">
+        <v>95.47</v>
+      </c>
+      <c r="K7" s="9">
+        <v>100</v>
+      </c>
+      <c r="L7" s="9">
+        <v>30</v>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="22">
+        <v>228</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9">
+        <v>20161017</v>
+      </c>
+      <c r="X7" s="23">
+        <v>20161017214202</v>
+      </c>
+      <c r="Y7" s="20">
+        <v>42660.903541666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9">
+        <v>50</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
+        <v>0.39993784999999998</v>
+      </c>
+      <c r="J8" s="22">
+        <v>1159.81</v>
+      </c>
+      <c r="K8" s="9">
+        <v>100</v>
+      </c>
+      <c r="L8" s="9">
+        <v>32</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="22">
+        <v>195</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9">
+        <v>20161017</v>
+      </c>
+      <c r="X8" s="23">
+        <v>20161017214202</v>
+      </c>
+      <c r="Y8" s="20">
+        <v>42660.903541666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9">
+        <v>72.484710000000007</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9">
+        <v>0.66990495000000005</v>
+      </c>
+      <c r="J9" s="22">
+        <v>-2059.71</v>
+      </c>
+      <c r="K9" s="9">
+        <v>100</v>
+      </c>
+      <c r="L9" s="9">
+        <v>-30</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="22">
+        <v>200</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9">
+        <v>20161017</v>
+      </c>
+      <c r="X9" s="23">
+        <v>20161017214202</v>
+      </c>
+      <c r="Y9" s="20">
+        <v>42660.903541666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>